<commit_message>
test include importe emissions
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BIEfIE/Boolean Include Emissions from Imported Electricity.xlsx
+++ b/InputData/ctrl-settings/BIEfIE/Boolean Include Emissions from Imported Electricity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\RMI_all_states\LA\ctrl-settings\BIEfIE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Louisiana\LA-eps\InputData\ctrl-settings\BIEfIE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0385FF5-E7F3-428B-89F4-954BEB65955A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C92B2F-569E-4A32-988D-7B6BDAF5DB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6825" yWindow="885" windowWidth="21945" windowHeight="15945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12615" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -528,7 +528,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>